<commit_message>
Added implementation to read the test data
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27514"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63D756A7-5F45-4859-AB51-025B4FDE1A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C38C9C3C-97C8-4944-9F13-B1AC1AB821CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>Module</t>
   </si>
@@ -42,20 +43,53 @@
     <t>ToBeExecuted</t>
   </si>
   <si>
-    <t>First_Test</t>
-  </si>
-  <si>
-    <t>TC_001_Check_First_Execution</t>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>TC_001_Verify_User_Able_To_Login_Successfully</t>
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://www.saucedemo.com/</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>standard_user</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Swag Labs</t>
+  </si>
+  <si>
+    <t>Logo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,8 +97,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -77,8 +126,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -123,17 +178,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -468,12 +545,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
     <col min="2" max="2" width="49.28515625" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" customWidth="1"/>
   </cols>
@@ -503,4 +581,93 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4128B6A2-E9C8-4D96-A4D7-D25A2A013B7B}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="52.5703125" customWidth="1"/>
+    <col min="2" max="2" width="52.85546875" customWidth="1"/>
+    <col min="3" max="3" width="67.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="'https://www.saucedemo.com/" xr:uid="{5E9B248B-AB96-4F05-A562-D2CC49ACFA3C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>